<commit_message>
changes: teacher_dashboard new fields and import and export for excel next update 3
</commit_message>
<xml_diff>
--- a/marks_template_10A.xlsx
+++ b/marks_template_10A.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,30 +429,25 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>roll_no</t>
+          <t>subject1</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>subject1</t>
+          <t>subject2</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>subject2</t>
+          <t>subject3</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>subject3</t>
+          <t>subject4</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
-        <is>
-          <t>subject4</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>subject5</t>
         </is>
@@ -464,16 +459,11 @@
           <t>Rahul</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -481,16 +471,11 @@
           <t>Aman</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -498,16 +483,11 @@
           <t>Neha</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -515,16 +495,11 @@
           <t>test</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>